<commit_message>
Office Changes for Create Order
</commit_message>
<xml_diff>
--- a/backend/importData/areaTable.xlsx
+++ b/backend/importData/areaTable.xlsx
@@ -1025,12 +1025,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="24.5703125" customWidth="1"/>
     <col min="7" max="7" width="13.7109375" customWidth="1"/>
     <col min="8" max="8" width="15.28515625" customWidth="1"/>
     <col min="9" max="9" width="9.7109375" customWidth="1"/>

</xml_diff>